<commit_message>
Chapter 9 Draft 1
</commit_message>
<xml_diff>
--- a/Virtues Spreadsheet.xlsx
+++ b/Virtues Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Dropbox\Documents\Books\A Study of the Aqdas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E357B8E-69AA-4CDE-B5C6-A89DEB7AA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE124AF-5B31-4780-9FEA-7FA99237C7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5A5C3805-CE89-4E01-8995-1F1F7BB0130C}"/>
   </bookViews>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552AABBD-5E21-4CC6-98D7-B9AA8D72861E}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Chapter 10 1st Draft
</commit_message>
<xml_diff>
--- a/Virtues Spreadsheet.xlsx
+++ b/Virtues Spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Dropbox\Documents\Books\A Study of the Aqdas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE124AF-5B31-4780-9FEA-7FA99237C7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81790D5E-3FDF-4A21-8537-95BCB376E891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5A5C3805-CE89-4E01-8995-1F1F7BB0130C}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552AABBD-5E21-4CC6-98D7-B9AA8D72861E}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Chapter 12 1st Draft
</commit_message>
<xml_diff>
--- a/Virtues Spreadsheet.xlsx
+++ b/Virtues Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Dropbox\Documents\Books\A Study of the Aqdas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C44D692-8111-42D2-947A-C7902CEF5502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE3BB5D-5F48-41B8-8D7A-88D5F4791EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5A5C3805-CE89-4E01-8995-1F1F7BB0130C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{5A5C3805-CE89-4E01-8995-1F1F7BB0130C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,10 +649,10 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
@@ -660,7 +660,7 @@
     <col min="4" max="4" width="54.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -674,7 +674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -688,7 +688,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -702,7 +702,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -716,7 +716,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -730,7 +730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -744,7 +744,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -758,7 +758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -772,7 +772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -786,7 +786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -814,7 +814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -828,7 +828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -856,7 +856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -870,7 +870,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -884,7 +884,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -898,7 +898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -912,7 +912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -926,7 +926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -940,7 +940,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -954,7 +954,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
@@ -968,7 +968,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -982,7 +982,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
@@ -996,7 +996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A26" s="5" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>

</xml_diff>